<commit_message>
Sskw: add column : Art
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskw_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskw_vorlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB17C017-A29F-458F-89FA-B4B8ACD0CF46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A40774C-6BE8-45A8-87BE-C693015A5464}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="32760" windowHeight="17145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sskw_Beispielbefüllung" sheetId="10" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sskw_Beispielbefüllung!$A$1:$Z$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sskw_Beispielbefüllung!$A$1:$AA$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sskw_Beispielbefüllung!$A:$B,Sskw_Beispielbefüllung!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <t>Isolierfall</t>
   </si>
@@ -214,6 +214,9 @@
   <si>
     <t>Prüf-
 kontakte</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -697,6 +700,15 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1038,34 +1050,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z120"/>
+  <dimension ref="A1:AA120"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:Z120"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="3" customWidth="1"/>
-    <col min="4" max="7" width="7.140625" style="3" customWidth="1"/>
-    <col min="8" max="9" width="5.5703125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="6" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="6" style="3" customWidth="1"/>
-    <col min="14" max="17" width="5.5703125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" style="3" customWidth="1"/>
-    <col min="19" max="22" width="5.5703125" style="3" customWidth="1"/>
-    <col min="23" max="23" width="12" style="3" customWidth="1"/>
-    <col min="24" max="24" width="4.140625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="10" style="3" customWidth="1"/>
-    <col min="26" max="26" width="10" style="25" customWidth="1"/>
-    <col min="27" max="16384" width="11.42578125" style="3"/>
+    <col min="3" max="3" width="5.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="3" customWidth="1"/>
+    <col min="5" max="8" width="7.140625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="5.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="6" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="6" style="3" customWidth="1"/>
+    <col min="15" max="18" width="5.5703125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="3" customWidth="1"/>
+    <col min="20" max="23" width="5.5703125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="12" style="3" customWidth="1"/>
+    <col min="25" max="25" width="4.140625" style="3" customWidth="1"/>
+    <col min="26" max="26" width="10" style="3" customWidth="1"/>
+    <col min="27" max="27" width="10" style="25" customWidth="1"/>
+    <col min="28" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16"/>
       <c r="B1" s="7" t="s">
         <v>10</v>
@@ -1142,217 +1155,226 @@
       <c r="Z1" s="7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="35" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="38"/>
       <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="35" t="s">
+      <c r="G2" s="38"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="39"/>
+      <c r="K2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="38"/>
       <c r="L2" s="38"/>
       <c r="M2" s="38"/>
       <c r="N2" s="38"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="34" t="s">
+      <c r="O2" s="38"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="34"/>
+      <c r="S2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="34" t="s">
+      <c r="T2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="34"/>
       <c r="U2" s="34"/>
       <c r="V2" s="34"/>
-      <c r="W2" s="34" t="s">
+      <c r="W2" s="34"/>
+      <c r="X2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="10" t="s">
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="Z2" s="10" t="s">
+      <c r="AA2" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="F3" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="41"/>
+      <c r="H3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="O3" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="42"/>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="42"/>
+      <c r="Q3" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="42"/>
+      <c r="S3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="T3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="V3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="X3" s="26" t="s">
+      <c r="Y3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="Y3" s="14" t="s">
+      <c r="Z3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="Z3" s="5"/>
-    </row>
-    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA3" s="5"/>
+    </row>
+    <row r="4" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="4"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="1"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="14"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="5"/>
-    </row>
-    <row r="5" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S4" s="14"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="5"/>
+    </row>
+    <row r="5" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="20"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="20"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="20" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="20"/>
+      <c r="N5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="O5" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="P5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="Q5" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="R5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="S5" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="S5" s="18" t="s">
+      <c r="T5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="T5" s="20"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="27"/>
-      <c r="Y5" s="22"/>
-      <c r="Z5" s="24"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U5" s="20"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="24"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="30"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="29"/>
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
       <c r="K6" s="30"/>
@@ -1370,13 +1392,14 @@
       <c r="W6" s="30"/>
       <c r="X6" s="30"/>
       <c r="Y6" s="30"/>
-      <c r="Z6" s="31"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z6" s="30"/>
+      <c r="AA6" s="31"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7" s="32"/>
-      <c r="E7" s="15"/>
+      <c r="C7" s="32"/>
       <c r="F7" s="15"/>
-      <c r="H7" s="15"/>
+      <c r="G7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
@@ -1394,361 +1417,363 @@
       <c r="W7" s="15"/>
       <c r="X7" s="15"/>
       <c r="Y7" s="15"/>
-      <c r="Z7" s="33"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z8" s="3"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z9" s="3"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z10" s="3"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z11" s="3"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z12" s="3"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z13" s="3"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z14" s="3"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z15" s="3"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z16" s="3"/>
-    </row>
-    <row r="17" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z17" s="3"/>
-    </row>
-    <row r="18" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z18" s="3"/>
-    </row>
-    <row r="19" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z19" s="3"/>
-    </row>
-    <row r="20" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z20" s="3"/>
-    </row>
-    <row r="21" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z21" s="3"/>
-    </row>
-    <row r="22" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z22" s="3"/>
-    </row>
-    <row r="23" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z23" s="3"/>
-    </row>
-    <row r="24" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z24" s="3"/>
-    </row>
-    <row r="25" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z25" s="3"/>
-    </row>
-    <row r="26" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z26" s="3"/>
-    </row>
-    <row r="27" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z27" s="3"/>
-    </row>
-    <row r="28" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z28" s="3"/>
-    </row>
-    <row r="29" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z29" s="3"/>
-    </row>
-    <row r="30" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z30" s="3"/>
-    </row>
-    <row r="31" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z31" s="3"/>
-    </row>
-    <row r="32" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z32" s="3"/>
-    </row>
-    <row r="33" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z33" s="3"/>
-    </row>
-    <row r="34" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z34" s="3"/>
-    </row>
-    <row r="35" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z35" s="3"/>
-    </row>
-    <row r="36" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z36" s="3"/>
-    </row>
-    <row r="37" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z37" s="3"/>
-    </row>
-    <row r="38" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z38" s="3"/>
-    </row>
-    <row r="39" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z39" s="3"/>
-    </row>
-    <row r="40" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z40" s="3"/>
-    </row>
-    <row r="41" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z41" s="3"/>
-    </row>
-    <row r="42" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z42" s="3"/>
-    </row>
-    <row r="43" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z43" s="3"/>
-    </row>
-    <row r="44" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z44" s="3"/>
-    </row>
-    <row r="45" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z45" s="3"/>
-    </row>
-    <row r="46" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z46" s="3"/>
-    </row>
-    <row r="47" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z47" s="3"/>
-    </row>
-    <row r="48" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z48" s="3"/>
-    </row>
-    <row r="49" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z49" s="3"/>
-    </row>
-    <row r="50" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z50" s="3"/>
-    </row>
-    <row r="51" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z51" s="3"/>
-    </row>
-    <row r="52" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z52" s="3"/>
-    </row>
-    <row r="53" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z53" s="3"/>
-    </row>
-    <row r="54" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z54" s="3"/>
-    </row>
-    <row r="55" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z55" s="3"/>
-    </row>
-    <row r="56" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z56" s="3"/>
-    </row>
-    <row r="57" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z57" s="3"/>
-    </row>
-    <row r="58" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z58" s="3"/>
-    </row>
-    <row r="59" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z59" s="3"/>
-    </row>
-    <row r="60" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z60" s="3"/>
-    </row>
-    <row r="61" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z61" s="3"/>
-    </row>
-    <row r="62" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z62" s="3"/>
-    </row>
-    <row r="63" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z63" s="3"/>
-    </row>
-    <row r="64" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z64" s="3"/>
-    </row>
-    <row r="65" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z65" s="3"/>
-    </row>
-    <row r="66" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z66" s="3"/>
-    </row>
-    <row r="67" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z67" s="3"/>
-    </row>
-    <row r="68" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z68" s="3"/>
-    </row>
-    <row r="69" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z69" s="3"/>
-    </row>
-    <row r="70" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z70" s="3"/>
-    </row>
-    <row r="71" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z71" s="3"/>
-    </row>
-    <row r="72" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z72" s="3"/>
-    </row>
-    <row r="73" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z73" s="3"/>
-    </row>
-    <row r="74" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z74" s="3"/>
-    </row>
-    <row r="75" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z75" s="3"/>
-    </row>
-    <row r="76" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z76" s="3"/>
-    </row>
-    <row r="77" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z77" s="3"/>
-    </row>
-    <row r="78" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z78" s="3"/>
-    </row>
-    <row r="79" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z79" s="3"/>
-    </row>
-    <row r="80" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z80" s="3"/>
-    </row>
-    <row r="81" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z81" s="3"/>
-    </row>
-    <row r="82" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z82" s="3"/>
-    </row>
-    <row r="83" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z83" s="3"/>
-    </row>
-    <row r="84" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z84" s="3"/>
-    </row>
-    <row r="85" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z85" s="3"/>
-    </row>
-    <row r="86" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z86" s="3"/>
-    </row>
-    <row r="87" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z87" s="3"/>
-    </row>
-    <row r="88" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z88" s="3"/>
-    </row>
-    <row r="89" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z89" s="3"/>
-    </row>
-    <row r="90" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z90" s="3"/>
-    </row>
-    <row r="91" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z91" s="3"/>
-    </row>
-    <row r="92" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z92" s="3"/>
-    </row>
-    <row r="93" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z93" s="3"/>
-    </row>
-    <row r="94" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z94" s="3"/>
-    </row>
-    <row r="95" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z95" s="3"/>
-    </row>
-    <row r="96" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z96" s="3"/>
-    </row>
-    <row r="97" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z97" s="3"/>
-    </row>
-    <row r="98" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z98" s="3"/>
-    </row>
-    <row r="99" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z99" s="3"/>
-    </row>
-    <row r="100" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z100" s="3"/>
-    </row>
-    <row r="101" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z101" s="3"/>
-    </row>
-    <row r="102" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z102" s="3"/>
-    </row>
-    <row r="103" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z103" s="3"/>
-    </row>
-    <row r="104" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z104" s="3"/>
-    </row>
-    <row r="105" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z105" s="3"/>
-    </row>
-    <row r="106" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z106" s="3"/>
-    </row>
-    <row r="107" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z107" s="3"/>
-    </row>
-    <row r="108" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z108" s="3"/>
-    </row>
-    <row r="109" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z109" s="3"/>
-    </row>
-    <row r="110" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z110" s="3"/>
-    </row>
-    <row r="111" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z111" s="3"/>
-    </row>
-    <row r="112" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z112" s="3"/>
-    </row>
-    <row r="113" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z113" s="3"/>
-    </row>
-    <row r="114" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z114" s="3"/>
-    </row>
-    <row r="115" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z115" s="3"/>
-    </row>
-    <row r="116" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z116" s="3"/>
-    </row>
-    <row r="117" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z117" s="3"/>
-    </row>
-    <row r="118" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z118" s="3"/>
-    </row>
-    <row r="119" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z119" s="3"/>
-    </row>
-    <row r="120" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z120" s="3"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="33"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA8" s="3"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA9" s="3"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA10" s="3"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA11" s="3"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA12" s="3"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA13" s="3"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA14" s="3"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA15" s="3"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA16" s="3"/>
+    </row>
+    <row r="17" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA17" s="3"/>
+    </row>
+    <row r="18" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA18" s="3"/>
+    </row>
+    <row r="19" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA19" s="3"/>
+    </row>
+    <row r="20" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA20" s="3"/>
+    </row>
+    <row r="21" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA21" s="3"/>
+    </row>
+    <row r="22" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA22" s="3"/>
+    </row>
+    <row r="23" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA23" s="3"/>
+    </row>
+    <row r="24" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA24" s="3"/>
+    </row>
+    <row r="25" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA25" s="3"/>
+    </row>
+    <row r="26" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA26" s="3"/>
+    </row>
+    <row r="27" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA27" s="3"/>
+    </row>
+    <row r="28" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA28" s="3"/>
+    </row>
+    <row r="29" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA29" s="3"/>
+    </row>
+    <row r="30" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA30" s="3"/>
+    </row>
+    <row r="31" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA31" s="3"/>
+    </row>
+    <row r="32" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA32" s="3"/>
+    </row>
+    <row r="33" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA33" s="3"/>
+    </row>
+    <row r="34" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA34" s="3"/>
+    </row>
+    <row r="35" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA35" s="3"/>
+    </row>
+    <row r="36" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA36" s="3"/>
+    </row>
+    <row r="37" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA37" s="3"/>
+    </row>
+    <row r="38" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA38" s="3"/>
+    </row>
+    <row r="39" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA39" s="3"/>
+    </row>
+    <row r="40" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA40" s="3"/>
+    </row>
+    <row r="41" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA41" s="3"/>
+    </row>
+    <row r="42" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA42" s="3"/>
+    </row>
+    <row r="43" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA43" s="3"/>
+    </row>
+    <row r="44" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA44" s="3"/>
+    </row>
+    <row r="45" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA45" s="3"/>
+    </row>
+    <row r="46" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA46" s="3"/>
+    </row>
+    <row r="47" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA47" s="3"/>
+    </row>
+    <row r="48" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA48" s="3"/>
+    </row>
+    <row r="49" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA49" s="3"/>
+    </row>
+    <row r="50" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA50" s="3"/>
+    </row>
+    <row r="51" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA51" s="3"/>
+    </row>
+    <row r="52" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA52" s="3"/>
+    </row>
+    <row r="53" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA53" s="3"/>
+    </row>
+    <row r="54" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA54" s="3"/>
+    </row>
+    <row r="55" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA55" s="3"/>
+    </row>
+    <row r="56" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA56" s="3"/>
+    </row>
+    <row r="57" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA57" s="3"/>
+    </row>
+    <row r="58" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA58" s="3"/>
+    </row>
+    <row r="59" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA59" s="3"/>
+    </row>
+    <row r="60" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA60" s="3"/>
+    </row>
+    <row r="61" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA61" s="3"/>
+    </row>
+    <row r="62" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA62" s="3"/>
+    </row>
+    <row r="63" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA63" s="3"/>
+    </row>
+    <row r="64" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA64" s="3"/>
+    </row>
+    <row r="65" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA65" s="3"/>
+    </row>
+    <row r="66" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA66" s="3"/>
+    </row>
+    <row r="67" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA67" s="3"/>
+    </row>
+    <row r="68" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA68" s="3"/>
+    </row>
+    <row r="69" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA69" s="3"/>
+    </row>
+    <row r="70" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA70" s="3"/>
+    </row>
+    <row r="71" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA71" s="3"/>
+    </row>
+    <row r="72" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA72" s="3"/>
+    </row>
+    <row r="73" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA73" s="3"/>
+    </row>
+    <row r="74" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA74" s="3"/>
+    </row>
+    <row r="75" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA75" s="3"/>
+    </row>
+    <row r="76" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA76" s="3"/>
+    </row>
+    <row r="77" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA77" s="3"/>
+    </row>
+    <row r="78" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA78" s="3"/>
+    </row>
+    <row r="79" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA79" s="3"/>
+    </row>
+    <row r="80" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA80" s="3"/>
+    </row>
+    <row r="81" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA81" s="3"/>
+    </row>
+    <row r="82" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA82" s="3"/>
+    </row>
+    <row r="83" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA83" s="3"/>
+    </row>
+    <row r="84" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA84" s="3"/>
+    </row>
+    <row r="85" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA85" s="3"/>
+    </row>
+    <row r="86" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA86" s="3"/>
+    </row>
+    <row r="87" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA87" s="3"/>
+    </row>
+    <row r="88" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA88" s="3"/>
+    </row>
+    <row r="89" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA89" s="3"/>
+    </row>
+    <row r="90" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA90" s="3"/>
+    </row>
+    <row r="91" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA91" s="3"/>
+    </row>
+    <row r="92" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA92" s="3"/>
+    </row>
+    <row r="93" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA93" s="3"/>
+    </row>
+    <row r="94" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA94" s="3"/>
+    </row>
+    <row r="95" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA95" s="3"/>
+    </row>
+    <row r="96" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA96" s="3"/>
+    </row>
+    <row r="97" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA97" s="3"/>
+    </row>
+    <row r="98" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA98" s="3"/>
+    </row>
+    <row r="99" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA99" s="3"/>
+    </row>
+    <row r="100" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA100" s="3"/>
+    </row>
+    <row r="101" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA101" s="3"/>
+    </row>
+    <row r="102" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA102" s="3"/>
+    </row>
+    <row r="103" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA103" s="3"/>
+    </row>
+    <row r="104" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA104" s="3"/>
+    </row>
+    <row r="105" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA105" s="3"/>
+    </row>
+    <row r="106" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA106" s="3"/>
+    </row>
+    <row r="107" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA107" s="3"/>
+    </row>
+    <row r="108" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA108" s="3"/>
+    </row>
+    <row r="109" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA109" s="3"/>
+    </row>
+    <row r="110" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA110" s="3"/>
+    </row>
+    <row r="111" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA111" s="3"/>
+    </row>
+    <row r="112" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA112" s="3"/>
+    </row>
+    <row r="113" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA113" s="3"/>
+    </row>
+    <row r="114" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA114" s="3"/>
+    </row>
+    <row r="115" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA115" s="3"/>
+    </row>
+    <row r="116" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA116" s="3"/>
+    </row>
+    <row r="117" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA117" s="3"/>
+    </row>
+    <row r="118" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA118" s="3"/>
+    </row>
+    <row r="119" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA119" s="3"/>
+    </row>
+    <row r="120" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA120" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W2:X2"/>
+  <mergeCells count="13">
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="X2:Y2"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="Q2:R2"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.19685039370078741" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -1756,15 +1781,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1956,7 +1972,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2002,19 +2031,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{200A6F7D-E42E-4B70-A15C-E8BEB8201794}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42480D0E-5E79-4221-80DC-2A0E463FB574}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2033,18 +2050,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{200A6F7D-E42E-4B70-A15C-E8BEB8201794}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A1226AB-A295-4535-9FC4-1666084BBC71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CDB2657-7114-41D8-B37C-6BEE1D3D81FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A1226AB-A295-4535-9FC4-1666084BBC71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sskw: add column : Art (#1150)
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskw_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskw_vorlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB17C017-A29F-458F-89FA-B4B8ACD0CF46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A40774C-6BE8-45A8-87BE-C693015A5464}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="32760" windowHeight="17145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sskw_Beispielbefüllung" sheetId="10" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sskw_Beispielbefüllung!$A$1:$Z$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sskw_Beispielbefüllung!$A$1:$AA$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sskw_Beispielbefüllung!$A:$B,Sskw_Beispielbefüllung!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <t>Isolierfall</t>
   </si>
@@ -214,6 +214,9 @@
   <si>
     <t>Prüf-
 kontakte</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -697,6 +700,15 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1038,34 +1050,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z120"/>
+  <dimension ref="A1:AA120"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:Z120"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="3" customWidth="1"/>
-    <col min="4" max="7" width="7.140625" style="3" customWidth="1"/>
-    <col min="8" max="9" width="5.5703125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="6" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="6" style="3" customWidth="1"/>
-    <col min="14" max="17" width="5.5703125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" style="3" customWidth="1"/>
-    <col min="19" max="22" width="5.5703125" style="3" customWidth="1"/>
-    <col min="23" max="23" width="12" style="3" customWidth="1"/>
-    <col min="24" max="24" width="4.140625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="10" style="3" customWidth="1"/>
-    <col min="26" max="26" width="10" style="25" customWidth="1"/>
-    <col min="27" max="16384" width="11.42578125" style="3"/>
+    <col min="3" max="3" width="5.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="3" customWidth="1"/>
+    <col min="5" max="8" width="7.140625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="5.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="6" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="6" style="3" customWidth="1"/>
+    <col min="15" max="18" width="5.5703125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="3" customWidth="1"/>
+    <col min="20" max="23" width="5.5703125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="12" style="3" customWidth="1"/>
+    <col min="25" max="25" width="4.140625" style="3" customWidth="1"/>
+    <col min="26" max="26" width="10" style="3" customWidth="1"/>
+    <col min="27" max="27" width="10" style="25" customWidth="1"/>
+    <col min="28" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16"/>
       <c r="B1" s="7" t="s">
         <v>10</v>
@@ -1142,217 +1155,226 @@
       <c r="Z1" s="7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="35" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="38"/>
       <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="35" t="s">
+      <c r="G2" s="38"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="39"/>
+      <c r="K2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="38"/>
       <c r="L2" s="38"/>
       <c r="M2" s="38"/>
       <c r="N2" s="38"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="34" t="s">
+      <c r="O2" s="38"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="34"/>
+      <c r="S2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="34" t="s">
+      <c r="T2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="34"/>
       <c r="U2" s="34"/>
       <c r="V2" s="34"/>
-      <c r="W2" s="34" t="s">
+      <c r="W2" s="34"/>
+      <c r="X2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="10" t="s">
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="Z2" s="10" t="s">
+      <c r="AA2" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="F3" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="41"/>
+      <c r="H3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="O3" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="42"/>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="42"/>
+      <c r="Q3" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="42"/>
+      <c r="S3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="T3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="V3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="X3" s="26" t="s">
+      <c r="Y3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="Y3" s="14" t="s">
+      <c r="Z3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="Z3" s="5"/>
-    </row>
-    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA3" s="5"/>
+    </row>
+    <row r="4" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="4"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="1"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="14"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="5"/>
-    </row>
-    <row r="5" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S4" s="14"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="5"/>
+    </row>
+    <row r="5" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="20"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="20"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="20" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="20"/>
+      <c r="N5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="O5" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="P5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="Q5" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="R5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="S5" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="S5" s="18" t="s">
+      <c r="T5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="T5" s="20"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="27"/>
-      <c r="Y5" s="22"/>
-      <c r="Z5" s="24"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U5" s="20"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="24"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="30"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="29"/>
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
       <c r="K6" s="30"/>
@@ -1370,13 +1392,14 @@
       <c r="W6" s="30"/>
       <c r="X6" s="30"/>
       <c r="Y6" s="30"/>
-      <c r="Z6" s="31"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z6" s="30"/>
+      <c r="AA6" s="31"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7" s="32"/>
-      <c r="E7" s="15"/>
+      <c r="C7" s="32"/>
       <c r="F7" s="15"/>
-      <c r="H7" s="15"/>
+      <c r="G7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
@@ -1394,361 +1417,363 @@
       <c r="W7" s="15"/>
       <c r="X7" s="15"/>
       <c r="Y7" s="15"/>
-      <c r="Z7" s="33"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z8" s="3"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z9" s="3"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z10" s="3"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z11" s="3"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z12" s="3"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z13" s="3"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z14" s="3"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z15" s="3"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z16" s="3"/>
-    </row>
-    <row r="17" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z17" s="3"/>
-    </row>
-    <row r="18" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z18" s="3"/>
-    </row>
-    <row r="19" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z19" s="3"/>
-    </row>
-    <row r="20" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z20" s="3"/>
-    </row>
-    <row r="21" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z21" s="3"/>
-    </row>
-    <row r="22" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z22" s="3"/>
-    </row>
-    <row r="23" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z23" s="3"/>
-    </row>
-    <row r="24" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z24" s="3"/>
-    </row>
-    <row r="25" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z25" s="3"/>
-    </row>
-    <row r="26" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z26" s="3"/>
-    </row>
-    <row r="27" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z27" s="3"/>
-    </row>
-    <row r="28" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z28" s="3"/>
-    </row>
-    <row r="29" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z29" s="3"/>
-    </row>
-    <row r="30" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z30" s="3"/>
-    </row>
-    <row r="31" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z31" s="3"/>
-    </row>
-    <row r="32" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z32" s="3"/>
-    </row>
-    <row r="33" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z33" s="3"/>
-    </row>
-    <row r="34" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z34" s="3"/>
-    </row>
-    <row r="35" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z35" s="3"/>
-    </row>
-    <row r="36" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z36" s="3"/>
-    </row>
-    <row r="37" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z37" s="3"/>
-    </row>
-    <row r="38" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z38" s="3"/>
-    </row>
-    <row r="39" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z39" s="3"/>
-    </row>
-    <row r="40" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z40" s="3"/>
-    </row>
-    <row r="41" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z41" s="3"/>
-    </row>
-    <row r="42" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z42" s="3"/>
-    </row>
-    <row r="43" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z43" s="3"/>
-    </row>
-    <row r="44" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z44" s="3"/>
-    </row>
-    <row r="45" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z45" s="3"/>
-    </row>
-    <row r="46" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z46" s="3"/>
-    </row>
-    <row r="47" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z47" s="3"/>
-    </row>
-    <row r="48" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z48" s="3"/>
-    </row>
-    <row r="49" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z49" s="3"/>
-    </row>
-    <row r="50" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z50" s="3"/>
-    </row>
-    <row r="51" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z51" s="3"/>
-    </row>
-    <row r="52" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z52" s="3"/>
-    </row>
-    <row r="53" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z53" s="3"/>
-    </row>
-    <row r="54" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z54" s="3"/>
-    </row>
-    <row r="55" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z55" s="3"/>
-    </row>
-    <row r="56" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z56" s="3"/>
-    </row>
-    <row r="57" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z57" s="3"/>
-    </row>
-    <row r="58" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z58" s="3"/>
-    </row>
-    <row r="59" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z59" s="3"/>
-    </row>
-    <row r="60" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z60" s="3"/>
-    </row>
-    <row r="61" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z61" s="3"/>
-    </row>
-    <row r="62" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z62" s="3"/>
-    </row>
-    <row r="63" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z63" s="3"/>
-    </row>
-    <row r="64" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z64" s="3"/>
-    </row>
-    <row r="65" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z65" s="3"/>
-    </row>
-    <row r="66" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z66" s="3"/>
-    </row>
-    <row r="67" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z67" s="3"/>
-    </row>
-    <row r="68" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z68" s="3"/>
-    </row>
-    <row r="69" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z69" s="3"/>
-    </row>
-    <row r="70" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z70" s="3"/>
-    </row>
-    <row r="71" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z71" s="3"/>
-    </row>
-    <row r="72" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z72" s="3"/>
-    </row>
-    <row r="73" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z73" s="3"/>
-    </row>
-    <row r="74" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z74" s="3"/>
-    </row>
-    <row r="75" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z75" s="3"/>
-    </row>
-    <row r="76" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z76" s="3"/>
-    </row>
-    <row r="77" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z77" s="3"/>
-    </row>
-    <row r="78" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z78" s="3"/>
-    </row>
-    <row r="79" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z79" s="3"/>
-    </row>
-    <row r="80" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z80" s="3"/>
-    </row>
-    <row r="81" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z81" s="3"/>
-    </row>
-    <row r="82" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z82" s="3"/>
-    </row>
-    <row r="83" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z83" s="3"/>
-    </row>
-    <row r="84" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z84" s="3"/>
-    </row>
-    <row r="85" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z85" s="3"/>
-    </row>
-    <row r="86" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z86" s="3"/>
-    </row>
-    <row r="87" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z87" s="3"/>
-    </row>
-    <row r="88" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z88" s="3"/>
-    </row>
-    <row r="89" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z89" s="3"/>
-    </row>
-    <row r="90" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z90" s="3"/>
-    </row>
-    <row r="91" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z91" s="3"/>
-    </row>
-    <row r="92" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z92" s="3"/>
-    </row>
-    <row r="93" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z93" s="3"/>
-    </row>
-    <row r="94" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z94" s="3"/>
-    </row>
-    <row r="95" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z95" s="3"/>
-    </row>
-    <row r="96" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z96" s="3"/>
-    </row>
-    <row r="97" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z97" s="3"/>
-    </row>
-    <row r="98" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z98" s="3"/>
-    </row>
-    <row r="99" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z99" s="3"/>
-    </row>
-    <row r="100" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z100" s="3"/>
-    </row>
-    <row r="101" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z101" s="3"/>
-    </row>
-    <row r="102" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z102" s="3"/>
-    </row>
-    <row r="103" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z103" s="3"/>
-    </row>
-    <row r="104" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z104" s="3"/>
-    </row>
-    <row r="105" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z105" s="3"/>
-    </row>
-    <row r="106" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z106" s="3"/>
-    </row>
-    <row r="107" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z107" s="3"/>
-    </row>
-    <row r="108" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z108" s="3"/>
-    </row>
-    <row r="109" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z109" s="3"/>
-    </row>
-    <row r="110" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z110" s="3"/>
-    </row>
-    <row r="111" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z111" s="3"/>
-    </row>
-    <row r="112" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z112" s="3"/>
-    </row>
-    <row r="113" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z113" s="3"/>
-    </row>
-    <row r="114" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z114" s="3"/>
-    </row>
-    <row r="115" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z115" s="3"/>
-    </row>
-    <row r="116" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z116" s="3"/>
-    </row>
-    <row r="117" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z117" s="3"/>
-    </row>
-    <row r="118" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z118" s="3"/>
-    </row>
-    <row r="119" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z119" s="3"/>
-    </row>
-    <row r="120" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z120" s="3"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="33"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA8" s="3"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA9" s="3"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA10" s="3"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA11" s="3"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA12" s="3"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA13" s="3"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA14" s="3"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA15" s="3"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA16" s="3"/>
+    </row>
+    <row r="17" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA17" s="3"/>
+    </row>
+    <row r="18" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA18" s="3"/>
+    </row>
+    <row r="19" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA19" s="3"/>
+    </row>
+    <row r="20" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA20" s="3"/>
+    </row>
+    <row r="21" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA21" s="3"/>
+    </row>
+    <row r="22" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA22" s="3"/>
+    </row>
+    <row r="23" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA23" s="3"/>
+    </row>
+    <row r="24" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA24" s="3"/>
+    </row>
+    <row r="25" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA25" s="3"/>
+    </row>
+    <row r="26" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA26" s="3"/>
+    </row>
+    <row r="27" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA27" s="3"/>
+    </row>
+    <row r="28" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA28" s="3"/>
+    </row>
+    <row r="29" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA29" s="3"/>
+    </row>
+    <row r="30" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA30" s="3"/>
+    </row>
+    <row r="31" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA31" s="3"/>
+    </row>
+    <row r="32" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA32" s="3"/>
+    </row>
+    <row r="33" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA33" s="3"/>
+    </row>
+    <row r="34" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA34" s="3"/>
+    </row>
+    <row r="35" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA35" s="3"/>
+    </row>
+    <row r="36" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA36" s="3"/>
+    </row>
+    <row r="37" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA37" s="3"/>
+    </row>
+    <row r="38" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA38" s="3"/>
+    </row>
+    <row r="39" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA39" s="3"/>
+    </row>
+    <row r="40" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA40" s="3"/>
+    </row>
+    <row r="41" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA41" s="3"/>
+    </row>
+    <row r="42" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA42" s="3"/>
+    </row>
+    <row r="43" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA43" s="3"/>
+    </row>
+    <row r="44" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA44" s="3"/>
+    </row>
+    <row r="45" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA45" s="3"/>
+    </row>
+    <row r="46" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA46" s="3"/>
+    </row>
+    <row r="47" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA47" s="3"/>
+    </row>
+    <row r="48" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA48" s="3"/>
+    </row>
+    <row r="49" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA49" s="3"/>
+    </row>
+    <row r="50" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA50" s="3"/>
+    </row>
+    <row r="51" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA51" s="3"/>
+    </row>
+    <row r="52" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA52" s="3"/>
+    </row>
+    <row r="53" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA53" s="3"/>
+    </row>
+    <row r="54" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA54" s="3"/>
+    </row>
+    <row r="55" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA55" s="3"/>
+    </row>
+    <row r="56" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA56" s="3"/>
+    </row>
+    <row r="57" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA57" s="3"/>
+    </row>
+    <row r="58" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA58" s="3"/>
+    </row>
+    <row r="59" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA59" s="3"/>
+    </row>
+    <row r="60" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA60" s="3"/>
+    </row>
+    <row r="61" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA61" s="3"/>
+    </row>
+    <row r="62" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA62" s="3"/>
+    </row>
+    <row r="63" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA63" s="3"/>
+    </row>
+    <row r="64" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA64" s="3"/>
+    </row>
+    <row r="65" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA65" s="3"/>
+    </row>
+    <row r="66" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA66" s="3"/>
+    </row>
+    <row r="67" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA67" s="3"/>
+    </row>
+    <row r="68" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA68" s="3"/>
+    </row>
+    <row r="69" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA69" s="3"/>
+    </row>
+    <row r="70" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA70" s="3"/>
+    </row>
+    <row r="71" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA71" s="3"/>
+    </row>
+    <row r="72" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA72" s="3"/>
+    </row>
+    <row r="73" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA73" s="3"/>
+    </row>
+    <row r="74" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA74" s="3"/>
+    </row>
+    <row r="75" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA75" s="3"/>
+    </row>
+    <row r="76" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA76" s="3"/>
+    </row>
+    <row r="77" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA77" s="3"/>
+    </row>
+    <row r="78" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA78" s="3"/>
+    </row>
+    <row r="79" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA79" s="3"/>
+    </row>
+    <row r="80" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA80" s="3"/>
+    </row>
+    <row r="81" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA81" s="3"/>
+    </row>
+    <row r="82" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA82" s="3"/>
+    </row>
+    <row r="83" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA83" s="3"/>
+    </row>
+    <row r="84" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA84" s="3"/>
+    </row>
+    <row r="85" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA85" s="3"/>
+    </row>
+    <row r="86" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA86" s="3"/>
+    </row>
+    <row r="87" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA87" s="3"/>
+    </row>
+    <row r="88" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA88" s="3"/>
+    </row>
+    <row r="89" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA89" s="3"/>
+    </row>
+    <row r="90" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA90" s="3"/>
+    </row>
+    <row r="91" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA91" s="3"/>
+    </row>
+    <row r="92" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA92" s="3"/>
+    </row>
+    <row r="93" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA93" s="3"/>
+    </row>
+    <row r="94" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA94" s="3"/>
+    </row>
+    <row r="95" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA95" s="3"/>
+    </row>
+    <row r="96" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA96" s="3"/>
+    </row>
+    <row r="97" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA97" s="3"/>
+    </row>
+    <row r="98" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA98" s="3"/>
+    </row>
+    <row r="99" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA99" s="3"/>
+    </row>
+    <row r="100" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA100" s="3"/>
+    </row>
+    <row r="101" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA101" s="3"/>
+    </row>
+    <row r="102" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA102" s="3"/>
+    </row>
+    <row r="103" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA103" s="3"/>
+    </row>
+    <row r="104" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA104" s="3"/>
+    </row>
+    <row r="105" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA105" s="3"/>
+    </row>
+    <row r="106" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA106" s="3"/>
+    </row>
+    <row r="107" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA107" s="3"/>
+    </row>
+    <row r="108" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA108" s="3"/>
+    </row>
+    <row r="109" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA109" s="3"/>
+    </row>
+    <row r="110" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA110" s="3"/>
+    </row>
+    <row r="111" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA111" s="3"/>
+    </row>
+    <row r="112" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA112" s="3"/>
+    </row>
+    <row r="113" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA113" s="3"/>
+    </row>
+    <row r="114" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA114" s="3"/>
+    </row>
+    <row r="115" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA115" s="3"/>
+    </row>
+    <row r="116" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA116" s="3"/>
+    </row>
+    <row r="117" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA117" s="3"/>
+    </row>
+    <row r="118" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA118" s="3"/>
+    </row>
+    <row r="119" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA119" s="3"/>
+    </row>
+    <row r="120" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA120" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W2:X2"/>
+  <mergeCells count="13">
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="X2:Y2"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="Q2:R2"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.19685039370078741" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -1756,15 +1781,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1956,7 +1972,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2002,19 +2031,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{200A6F7D-E42E-4B70-A15C-E8BEB8201794}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42480D0E-5E79-4221-80DC-2A0E463FB574}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2033,18 +2050,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{200A6F7D-E42E-4B70-A15C-E8BEB8201794}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A1226AB-A295-4535-9FC4-1666084BBC71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CDB2657-7114-41D8-B37C-6BEE1D3D81FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A1226AB-A295-4535-9FC4-1666084BBC71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sskw - extend pruefkontakte column header (#2199)
* update excel template

* update table references
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskw_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskw_vorlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws_intern\planpro\set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws_intern\planpro\repos\set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCECE363-3104-49F5-99A1-91E73B060C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B035B7FB-A7FF-4185-8730-161EC0D5E553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="50820" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sskw_Beispielbefüllung" sheetId="10" r:id="rId1"/>
@@ -212,11 +212,12 @@
     <t>Anzahl (Lage) Antriebe</t>
   </si>
   <si>
+    <t>Z</t>
+  </si>
+  <si>
     <t>Prüf-
-kontakte</t>
-  </si>
-  <si>
-    <t>Z</t>
+kontakte
+(Zprk)</t>
   </si>
 </sst>
 </file>
@@ -478,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -534,6 +535,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -541,30 +560,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -874,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA120"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -978,76 +973,76 @@
         <v>50</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="27" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="27" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="27" t="s">
+      <c r="J2" s="24"/>
+      <c r="K2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="27" t="s">
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="29"/>
+      <c r="R2" s="24"/>
       <c r="S2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="T2" s="27" t="s">
+      <c r="T2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="27" t="s">
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="Y2" s="29"/>
+      <c r="Y2" s="24"/>
       <c r="Z2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AA2" s="24" t="s">
+      <c r="AA2" s="19" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:27" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="26" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="21"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1067,16 +1062,16 @@
         <v>47</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="19" t="s">
+      <c r="P3" s="26"/>
+      <c r="Q3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="R3" s="20"/>
+      <c r="R3" s="26"/>
       <c r="S3" s="10" t="s">
         <v>58</v>
       </c>
@@ -1101,13 +1096,13 @@
       <c r="Z3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="AA3" s="25"/>
+      <c r="AA3" s="20"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="20"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="1"/>
       <c r="F4" s="4" t="s">
         <v>41</v>
@@ -1142,7 +1137,7 @@
       <c r="X4" s="1"/>
       <c r="Y4" s="5"/>
       <c r="Z4" s="10"/>
-      <c r="AA4" s="25"/>
+      <c r="AA4" s="20"/>
     </row>
     <row r="5" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
@@ -1187,35 +1182,12 @@
       <c r="X5" s="13"/>
       <c r="Y5" s="14"/>
       <c r="Z5" s="16"/>
-      <c r="AA5" s="26"/>
+      <c r="AA5" s="21"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="22"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="AA6" s="18"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7" s="18"/>
@@ -1583,10 +1555,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1595,7 +1563,57 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1787,53 +1805,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{200A6F7D-E42E-4B70-A15C-E8BEB8201794}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A1226AB-A295-4535-9FC4-1666084BBC71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
@@ -1841,15 +1821,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{200A6F7D-E42E-4B70-A15C-E8BEB8201794}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CDB2657-7114-41D8-B37C-6BEE1D3D81FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42480D0E-5E79-4221-80DC-2A0E463FB574}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1866,12 +1846,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CDB2657-7114-41D8-B37C-6BEE1D3D81FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>